<commit_message>
Cash flow output values, the first few.
</commit_message>
<xml_diff>
--- a/WhenToMine.xlsx
+++ b/WhenToMine.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="1680" windowWidth="23920" windowHeight="12260" tabRatio="500"/>
+    <workbookView xWindow="5940" yWindow="1560" windowWidth="23920" windowHeight="12260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,12 +66,6 @@
     <t>kWh / GHash</t>
   </si>
   <si>
-    <t>Watt / GHash</t>
-  </si>
-  <si>
-    <t>kWh / Watt</t>
-  </si>
-  <si>
     <t>pool fee %</t>
   </si>
   <si>
@@ -316,22 +310,29 @@
   </si>
   <si>
     <t>- electricity cost</t>
+  </si>
+  <si>
+    <t>WattHour / GHash</t>
+  </si>
+  <si>
+    <t>kW / Watt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="9">
+  <numFmts count="10">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
     <numFmt numFmtId="166" formatCode="#,##0.000000"/>
-    <numFmt numFmtId="168" formatCode="0.0E+00"/>
-    <numFmt numFmtId="169" formatCode="0.0.E+00"/>
-    <numFmt numFmtId="171" formatCode="#,##0.00000"/>
-    <numFmt numFmtId="173" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
-    <numFmt numFmtId="175" formatCode="0%;[Red]\-0%"/>
-    <numFmt numFmtId="176" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
+    <numFmt numFmtId="167" formatCode="0.0E+00"/>
+    <numFmt numFmtId="168" formatCode="0.0.E+00"/>
+    <numFmt numFmtId="169" formatCode="#,##0.00000"/>
+    <numFmt numFmtId="170" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
+    <numFmt numFmtId="171" formatCode="0%;[Red]\-0%"/>
+    <numFmt numFmtId="172" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
+    <numFmt numFmtId="173" formatCode="0.000000E+00"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -563,7 +564,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="298">
+  <cellStyleXfs count="312">
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -862,6 +863,20 @@
     <xf numFmtId="3" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="3" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="83">
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -883,13 +898,12 @@
     <xf numFmtId="166" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -904,10 +918,10 @@
     <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -959,9 +973,9 @@
     <xf numFmtId="9" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -979,10 +993,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="6" fillId="0" borderId="0" xfId="197" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" xfId="197" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -991,8 +1005,9 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
+    <xf numFmtId="173" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="298">
+  <cellStyles count="312">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1141,6 +1156,13 @@
     <cellStyle name="Followed Hyperlink" xfId="293" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="295" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="297" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="299" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="301" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="303" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="305" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="307" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="309" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="311" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1289,6 +1311,13 @@
     <cellStyle name="Hyperlink" xfId="292" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="294" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="296" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="298" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="300" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="302" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="304" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="306" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="308" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="310" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Percent" xfId="197" builtinId="5"/>
   </cellStyles>
@@ -1621,112 +1650,112 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I126"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="31.1640625" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="33.5" style="28" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="3" max="3" width="33.5" style="27" customWidth="1"/>
     <col min="4" max="4" width="3.83203125" customWidth="1"/>
     <col min="5" max="5" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18">
-      <c r="A1" s="62" t="s">
-        <v>51</v>
+      <c r="A1" s="61" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="23" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="40"/>
+      <c r="C5" s="39"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="64" t="s">
-        <v>94</v>
+      <c r="A6" s="63" t="s">
+        <v>92</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="41"/>
+      <c r="C6" s="40"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="64"/>
+      <c r="A7" s="63"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="41"/>
+      <c r="C7" s="40"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="34">
-        <v>550</v>
-      </c>
-      <c r="C8" s="41" t="s">
+      <c r="B8" s="33">
+        <v>123</v>
+      </c>
+      <c r="C8" s="40" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="25" t="s">
-        <v>31</v>
+      <c r="A9" s="24" t="s">
+        <v>29</v>
       </c>
       <c r="B9" s="12">
         <f>60*60</f>
         <v>3600</v>
       </c>
-      <c r="C9" s="41" t="s">
+      <c r="C9" s="40" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="53" t="s">
-        <v>27</v>
+      <c r="A10" s="52" t="s">
+        <v>25</v>
       </c>
       <c r="B10" s="15">
         <f>B8*B9</f>
-        <v>1980000</v>
-      </c>
-      <c r="C10" s="41" t="s">
+        <v>442800</v>
+      </c>
+      <c r="C10" s="40" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="5"/>
       <c r="B11" s="2"/>
-      <c r="C11" s="41"/>
+      <c r="C11" s="40"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="41" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="7">
-        <v>4000</v>
-      </c>
-      <c r="C12" s="41" t="s">
+        <v>337</v>
+      </c>
+      <c r="C12" s="40" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="43" t="s">
-        <v>23</v>
+      <c r="A13" s="42" t="s">
+        <v>21</v>
       </c>
       <c r="B13" s="9">
-        <v>0</v>
-      </c>
-      <c r="C13" s="41" t="s">
+        <v>9999</v>
+      </c>
+      <c r="C13" s="40" t="s">
         <v>0</v>
       </c>
       <c r="E13" t="s">
@@ -1734,368 +1763,368 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="26" t="s">
-        <v>26</v>
+      <c r="A14" s="25" t="s">
+        <v>24</v>
       </c>
       <c r="B14" s="2">
         <f>B12+B13</f>
-        <v>4000</v>
-      </c>
-      <c r="C14" s="41" t="s">
+        <v>10336</v>
+      </c>
+      <c r="C14" s="40" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="5"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="41"/>
+      <c r="C15" s="40"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="41" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="2">
         <f>B14</f>
-        <v>4000</v>
-      </c>
-      <c r="C16" s="41" t="s">
+        <v>10336</v>
+      </c>
+      <c r="C16" s="40" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="43" t="s">
-        <v>24</v>
+      <c r="A17" s="42" t="s">
+        <v>22</v>
       </c>
       <c r="B17" s="2">
         <f>B10</f>
-        <v>1980000</v>
-      </c>
-      <c r="C17" s="41" t="s">
+        <v>442800</v>
+      </c>
+      <c r="C17" s="40" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="26" t="s">
-        <v>28</v>
+      <c r="A18" s="25" t="s">
+        <v>26</v>
       </c>
       <c r="B18" s="13">
         <f>B16/B17</f>
-        <v>2.0202020202020202E-3</v>
-      </c>
-      <c r="C18" s="41" t="s">
-        <v>15</v>
+        <v>2.3342366757000903E-2</v>
+      </c>
+      <c r="C18" s="40" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="26" t="s">
-        <v>31</v>
+      <c r="A19" s="25" t="s">
+        <v>29</v>
       </c>
       <c r="B19" s="14">
         <f>1/1000</f>
         <v>1E-3</v>
       </c>
-      <c r="C19" s="41" t="s">
-        <v>16</v>
+      <c r="C19" s="40" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="17">
+      <c r="A20" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="82">
         <f>B18*B19</f>
-        <v>2.0202020202020202E-6</v>
-      </c>
-      <c r="C20" s="41" t="s">
+        <v>2.3342366757000903E-5</v>
+      </c>
+      <c r="C20" s="40" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="47"/>
+      <c r="A21" s="46"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="48"/>
+      <c r="C21" s="47"/>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
-      <c r="C22" s="29"/>
+      <c r="C22" s="28"/>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
-      <c r="C23" s="29"/>
+      <c r="C23" s="28"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="24" t="s">
-        <v>53</v>
+      <c r="A24" s="23" t="s">
+        <v>51</v>
       </c>
       <c r="B24" s="4"/>
-      <c r="C24" s="40"/>
+      <c r="C24" s="39"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="64" t="s">
-        <v>95</v>
+      <c r="A25" s="63" t="s">
+        <v>93</v>
       </c>
       <c r="B25" s="2"/>
-      <c r="C25" s="41"/>
+      <c r="C25" s="40"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="64"/>
+      <c r="A26" s="63"/>
       <c r="B26" s="2"/>
-      <c r="C26" s="41"/>
+      <c r="C26" s="40"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="B27" s="20">
+      <c r="A27" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="19">
         <v>1180923195.2579999</v>
       </c>
-      <c r="C27" s="41"/>
+      <c r="C27" s="40"/>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="43" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" s="32">
+      <c r="A28" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="31">
         <f>2^256</f>
         <v>1.157920892373162E+77</v>
       </c>
-      <c r="C28" s="41" t="s">
+      <c r="C28" s="40" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="42" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="43" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" s="32">
+      <c r="B29" s="31">
         <f xml:space="preserve"> HEX2DEC("ffff") * 2^208</f>
         <v>2.6959535291011309E+67</v>
       </c>
-      <c r="C29" s="41" t="s">
-        <v>36</v>
+      <c r="C29" s="40" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30" s="19">
+      <c r="A30" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="18">
         <f>B27*B28/B29</f>
         <v>5.0721038968843971E+18</v>
       </c>
-      <c r="C30" s="41" t="s">
-        <v>35</v>
+      <c r="C30" s="40" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" s="35">
+      <c r="A31" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="34">
         <f>1/1000000000</f>
         <v>1.0000000000000001E-9</v>
       </c>
-      <c r="C31" s="41" t="s">
-        <v>43</v>
+      <c r="C31" s="40" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="49" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="19">
+      <c r="A32" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" s="18">
         <f>B30*B31</f>
         <v>5072103896.8843975</v>
       </c>
-      <c r="C32" s="41"/>
+      <c r="C32" s="40"/>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="5"/>
       <c r="B33" s="2"/>
-      <c r="C33" s="41"/>
+      <c r="C33" s="40"/>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="42" t="s">
-        <v>19</v>
+      <c r="A34" s="41" t="s">
+        <v>17</v>
       </c>
       <c r="B34" s="10">
         <v>25</v>
       </c>
-      <c r="C34" s="41" t="s">
-        <v>21</v>
+      <c r="C34" s="40" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="43" t="s">
-        <v>30</v>
-      </c>
-      <c r="B35" s="22">
+      <c r="A35" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35" s="21">
         <f>B32</f>
         <v>5072103896.8843975</v>
       </c>
-      <c r="C35" s="41" t="s">
-        <v>20</v>
+      <c r="C35" s="40" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="44" t="s">
-        <v>41</v>
-      </c>
-      <c r="B36" s="33">
+      <c r="A36" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="32">
         <f>B34/B35</f>
         <v>4.9289211160198352E-9</v>
       </c>
-      <c r="C36" s="41" t="s">
-        <v>22</v>
+      <c r="C36" s="40" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="B37" s="31">
+      <c r="A37" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="30">
         <f>B10</f>
-        <v>1980000</v>
-      </c>
-      <c r="C37" s="41" t="s">
+        <v>442800</v>
+      </c>
+      <c r="C37" s="40" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="50" t="s">
-        <v>55</v>
-      </c>
-      <c r="B38" s="23">
+      <c r="A38" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" s="22">
         <f>B36*B37</f>
-        <v>9.7592638097192732E-3</v>
-      </c>
-      <c r="C38" s="45" t="s">
-        <v>34</v>
+        <v>2.1825262701735829E-3</v>
+      </c>
+      <c r="C38" s="44" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="47"/>
+      <c r="A39" s="46"/>
       <c r="B39" s="6"/>
-      <c r="C39" s="48"/>
+      <c r="C39" s="47"/>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
-      <c r="C40" s="29"/>
+      <c r="C40" s="28"/>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="B42" s="21"/>
-      <c r="C42" s="40"/>
+      <c r="A42" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="B42" s="20"/>
+      <c r="C42" s="39"/>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="64" t="s">
-        <v>62</v>
-      </c>
-      <c r="B43" s="22"/>
-      <c r="C43" s="41"/>
+      <c r="A43" s="63" t="s">
+        <v>60</v>
+      </c>
+      <c r="B43" s="21"/>
+      <c r="C43" s="40"/>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="64" t="s">
-        <v>71</v>
+      <c r="A44" s="63" t="s">
+        <v>69</v>
       </c>
       <c r="B44" s="2"/>
-      <c r="C44" s="41"/>
+      <c r="C44" s="40"/>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="5"/>
       <c r="B45" s="2"/>
-      <c r="C45" s="41"/>
+      <c r="C45" s="40"/>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="B46" s="22">
+      <c r="A46" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46" s="21">
         <f>B38</f>
-        <v>9.7592638097192732E-3</v>
-      </c>
-      <c r="C46" s="41" t="s">
-        <v>34</v>
+        <v>2.1825262701735829E-3</v>
+      </c>
+      <c r="C46" s="40" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" s="26" t="s">
-        <v>39</v>
+      <c r="A47" s="25" t="s">
+        <v>37</v>
       </c>
       <c r="B47" s="12">
-        <v>678</v>
-      </c>
-      <c r="C47" s="41" t="s">
-        <v>40</v>
+        <v>760</v>
+      </c>
+      <c r="C47" s="40" t="s">
+        <v>38</v>
       </c>
       <c r="E47" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="B48" s="65">
+      <c r="A48" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="B48" s="64">
         <f>B38*B47</f>
-        <v>6.6167808629896676</v>
-      </c>
-      <c r="C48" s="41" t="s">
+        <v>1.6587199653319229</v>
+      </c>
+      <c r="C48" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="D48" s="37"/>
+      <c r="D48" s="36"/>
       <c r="E48" t="s">
-        <v>78</v>
-      </c>
-      <c r="F48" s="63"/>
+        <v>76</v>
+      </c>
+      <c r="F48" s="62"/>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="27"/>
-      <c r="B49" s="68"/>
-      <c r="C49" s="48"/>
+      <c r="A49" s="26"/>
+      <c r="B49" s="67"/>
+      <c r="C49" s="47"/>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="8"/>
-      <c r="B50" s="36"/>
-      <c r="C50" s="29"/>
+      <c r="B50" s="35"/>
+      <c r="C50" s="28"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="24" t="s">
-        <v>58</v>
+      <c r="A52" s="23" t="s">
+        <v>56</v>
       </c>
       <c r="B52" s="4"/>
-      <c r="C52" s="40"/>
+      <c r="C52" s="39"/>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="64" t="s">
-        <v>96</v>
+      <c r="A53" s="63" t="s">
+        <v>94</v>
       </c>
       <c r="B53" s="2"/>
-      <c r="C53" s="41"/>
+      <c r="C53" s="40"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="5"/>
       <c r="B54" s="2"/>
-      <c r="C54" s="41"/>
+      <c r="C54" s="40"/>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="51" t="s">
-        <v>87</v>
-      </c>
-      <c r="B55" s="18">
+      <c r="A55" s="50" t="s">
+        <v>85</v>
+      </c>
+      <c r="B55" s="17">
         <f>0.15/0.6</f>
         <v>0.25</v>
       </c>
-      <c r="C55" s="45" t="s">
+      <c r="C55" s="44" t="s">
         <v>3</v>
       </c>
       <c r="E55" t="s">
@@ -2103,527 +2132,527 @@
       </c>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="26" t="s">
-        <v>32</v>
+      <c r="A56" s="25" t="s">
+        <v>30</v>
       </c>
       <c r="B56" s="2">
         <f>B20</f>
-        <v>2.0202020202020202E-6</v>
-      </c>
-      <c r="C56" s="41" t="s">
+        <v>2.3342366757000903E-5</v>
+      </c>
+      <c r="C56" s="40" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="57" spans="1:5">
-      <c r="A57" s="52" t="s">
-        <v>33</v>
+      <c r="A57" s="51" t="s">
+        <v>31</v>
       </c>
       <c r="B57" s="2">
         <f>B10</f>
-        <v>1980000</v>
-      </c>
-      <c r="C57" s="41" t="s">
+        <v>442800</v>
+      </c>
+      <c r="C57" s="40" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:5">
-      <c r="A58" s="46" t="s">
-        <v>59</v>
+      <c r="A58" s="45" t="s">
+        <v>57</v>
       </c>
       <c r="B58" s="16">
         <f>B55*B56*B57</f>
-        <v>1</v>
-      </c>
-      <c r="C58" s="41" t="s">
+        <v>2.5840000000000001</v>
+      </c>
+      <c r="C58" s="40" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="51"/>
+      <c r="A59" s="50"/>
       <c r="B59" s="2"/>
-      <c r="C59" s="41"/>
+      <c r="C59" s="40"/>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="51"/>
+      <c r="A60" s="50"/>
       <c r="B60" s="2"/>
-      <c r="C60" s="41"/>
+      <c r="C60" s="40"/>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="B61" s="60">
+      <c r="A61" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="B61" s="59">
         <v>0</v>
       </c>
-      <c r="C61" s="45"/>
+      <c r="C61" s="44"/>
     </row>
     <row r="62" spans="1:5">
-      <c r="A62" s="52" t="s">
-        <v>57</v>
-      </c>
-      <c r="B62" s="22">
+      <c r="A62" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="B62" s="21">
         <f>B38</f>
-        <v>9.7592638097192732E-3</v>
-      </c>
-      <c r="C62" s="41" t="s">
-        <v>34</v>
+        <v>2.1825262701735829E-3</v>
+      </c>
+      <c r="C62" s="40" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="63" spans="1:5">
-      <c r="A63" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="B63" s="23">
+      <c r="A63" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="B63" s="22">
         <f>B62*B61</f>
         <v>0</v>
       </c>
-      <c r="C63" s="41" t="s">
-        <v>34</v>
+      <c r="C63" s="40" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="64" spans="1:5">
-      <c r="A64" s="61"/>
+      <c r="A64" s="60"/>
       <c r="B64" s="2"/>
-      <c r="C64" s="41"/>
+      <c r="C64" s="40"/>
     </row>
     <row r="65" spans="1:5">
-      <c r="A65" s="61"/>
+      <c r="A65" s="60"/>
       <c r="B65" s="2"/>
-      <c r="C65" s="41"/>
+      <c r="C65" s="40"/>
     </row>
     <row r="66" spans="1:5">
-      <c r="A66" s="25" t="s">
-        <v>60</v>
+      <c r="A66" s="24" t="s">
+        <v>58</v>
       </c>
       <c r="B66" s="11">
         <v>0</v>
       </c>
-      <c r="C66" s="41" t="s">
+      <c r="C66" s="40" t="s">
         <v>8</v>
       </c>
       <c r="E66" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="67" spans="1:5">
-      <c r="A67" s="25" t="s">
-        <v>48</v>
+      <c r="A67" s="24" t="s">
+        <v>46</v>
       </c>
       <c r="B67" s="11">
         <v>0</v>
       </c>
-      <c r="C67" s="41" t="s">
+      <c r="C67" s="40" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="68" spans="1:5">
-      <c r="A68" s="53" t="s">
-        <v>49</v>
+      <c r="A68" s="52" t="s">
+        <v>47</v>
       </c>
       <c r="B68" s="15">
         <f>B66+B67</f>
         <v>0</v>
       </c>
-      <c r="C68" s="41" t="s">
+      <c r="C68" s="40" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="69" spans="1:5">
-      <c r="A69" s="47"/>
+      <c r="A69" s="46"/>
       <c r="B69" s="6"/>
-      <c r="C69" s="48"/>
+      <c r="C69" s="47"/>
     </row>
     <row r="72" spans="1:5">
-      <c r="A72" s="39" t="s">
-        <v>85</v>
-      </c>
-      <c r="B72" s="69"/>
-      <c r="C72" s="40"/>
+      <c r="A72" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="B72" s="68"/>
+      <c r="C72" s="39"/>
     </row>
     <row r="73" spans="1:5">
-      <c r="A73" s="64" t="s">
-        <v>69</v>
-      </c>
-      <c r="B73" s="36"/>
-      <c r="C73" s="41"/>
+      <c r="A73" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="B73" s="35"/>
+      <c r="C73" s="40"/>
     </row>
     <row r="74" spans="1:5">
-      <c r="A74" s="64" t="s">
-        <v>70</v>
-      </c>
-      <c r="B74" s="36"/>
-      <c r="C74" s="41"/>
+      <c r="A74" s="63" t="s">
+        <v>68</v>
+      </c>
+      <c r="B74" s="35"/>
+      <c r="C74" s="40"/>
     </row>
     <row r="75" spans="1:5">
-      <c r="A75" s="64"/>
-      <c r="B75" s="36"/>
-      <c r="C75" s="41"/>
+      <c r="A75" s="63"/>
+      <c r="B75" s="35"/>
+      <c r="C75" s="40"/>
     </row>
     <row r="76" spans="1:5">
-      <c r="A76" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="B76" s="36">
+      <c r="A76" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="B76" s="35">
         <f>B63</f>
         <v>0</v>
       </c>
-      <c r="C76" s="41" t="s">
-        <v>34</v>
+      <c r="C76" s="40" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="77" spans="1:5">
-      <c r="A77" s="43" t="s">
-        <v>39</v>
+      <c r="A77" s="42" t="s">
+        <v>37</v>
       </c>
       <c r="B77" s="3">
         <f>B47</f>
-        <v>678</v>
-      </c>
-      <c r="C77" s="41" t="s">
-        <v>40</v>
+        <v>760</v>
+      </c>
+      <c r="C77" s="40" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="78" spans="1:5">
-      <c r="A78" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="B78" s="38">
+      <c r="A78" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="B78" s="37">
         <f>B51*B77</f>
         <v>0</v>
       </c>
-      <c r="C78" s="41" t="s">
+      <c r="C78" s="40" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="79" spans="1:5">
-      <c r="A79" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="B79" s="36">
+      <c r="A79" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="B79" s="35">
         <f>B58</f>
-        <v>1</v>
-      </c>
-      <c r="C79" s="41" t="s">
+        <v>2.5840000000000001</v>
+      </c>
+      <c r="C79" s="40" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="80" spans="1:5">
-      <c r="A80" s="54" t="s">
-        <v>84</v>
-      </c>
-      <c r="B80" s="38">
+      <c r="A80" s="53" t="s">
+        <v>82</v>
+      </c>
+      <c r="B80" s="37">
         <f>B78+B79</f>
-        <v>1</v>
-      </c>
-      <c r="C80" s="41" t="s">
+        <v>2.5840000000000001</v>
+      </c>
+      <c r="C80" s="40" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:5">
-      <c r="A81" s="70"/>
-      <c r="B81" s="71"/>
-      <c r="C81" s="48"/>
+      <c r="A81" s="69"/>
+      <c r="B81" s="70"/>
+      <c r="C81" s="47"/>
     </row>
     <row r="82" spans="1:5">
-      <c r="A82" s="66"/>
-      <c r="B82" s="55"/>
-      <c r="C82" s="29"/>
+      <c r="A82" s="65"/>
+      <c r="B82" s="54"/>
+      <c r="C82" s="28"/>
     </row>
     <row r="83" spans="1:5">
-      <c r="A83" s="66"/>
-      <c r="B83" s="55"/>
-      <c r="C83" s="29"/>
+      <c r="A83" s="65"/>
+      <c r="B83" s="54"/>
+      <c r="C83" s="28"/>
     </row>
     <row r="84" spans="1:5">
-      <c r="A84" s="72" t="s">
-        <v>61</v>
-      </c>
-      <c r="B84" s="58"/>
-      <c r="C84" s="40"/>
+      <c r="A84" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="B84" s="57"/>
+      <c r="C84" s="39"/>
     </row>
     <row r="85" spans="1:5">
-      <c r="A85" s="73" t="s">
+      <c r="A85" s="72" t="s">
+        <v>70</v>
+      </c>
+      <c r="B85" s="54"/>
+      <c r="C85" s="40"/>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" s="72" t="s">
         <v>72</v>
       </c>
-      <c r="B85" s="55"/>
-      <c r="C85" s="41"/>
-    </row>
-    <row r="86" spans="1:5">
-      <c r="A86" s="73" t="s">
+      <c r="B86" s="54"/>
+      <c r="C86" s="40"/>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" s="53"/>
+      <c r="B87" s="54"/>
+      <c r="C87" s="40"/>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="B88" s="73">
+        <f>B48</f>
+        <v>1.6587199653319229</v>
+      </c>
+      <c r="C88" s="40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" s="55" t="s">
+        <v>87</v>
+      </c>
+      <c r="B89" s="73">
+        <f>B80</f>
+        <v>2.5840000000000001</v>
+      </c>
+      <c r="C89" s="40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="B90" s="74">
+        <f>B88-B89</f>
+        <v>-0.92528003466807718</v>
+      </c>
+      <c r="C90" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="E90" s="36"/>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B91" s="75">
+        <f>B90/B88</f>
+        <v>-0.55782775514064631</v>
+      </c>
+      <c r="C91" s="40"/>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" s="69"/>
+      <c r="B92" s="70"/>
+      <c r="C92" s="47"/>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" s="65"/>
+      <c r="B93" s="54"/>
+      <c r="C93" s="28"/>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" s="65"/>
+      <c r="B94" s="54"/>
+      <c r="C94" s="28"/>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" s="71" t="s">
+        <v>95</v>
+      </c>
+      <c r="B95" s="57"/>
+      <c r="C95" s="39"/>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" s="72" t="s">
+        <v>73</v>
+      </c>
+      <c r="B96" s="54"/>
+      <c r="C96" s="40"/>
+    </row>
+    <row r="97" spans="1:9">
+      <c r="A97" s="72" t="s">
         <v>74</v>
       </c>
-      <c r="B86" s="55"/>
-      <c r="C86" s="41"/>
-    </row>
-    <row r="87" spans="1:5">
-      <c r="A87" s="54"/>
-      <c r="B87" s="55"/>
-      <c r="C87" s="41"/>
-    </row>
-    <row r="88" spans="1:5">
-      <c r="A88" s="56" t="s">
-        <v>66</v>
-      </c>
-      <c r="B88" s="74">
-        <f>B48</f>
-        <v>6.6167808629896676</v>
-      </c>
-      <c r="C88" s="41" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5">
-      <c r="A89" s="56" t="s">
-        <v>89</v>
-      </c>
-      <c r="B89" s="74">
-        <f>B80</f>
-        <v>1</v>
-      </c>
-      <c r="C89" s="41" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5">
-      <c r="A90" s="54" t="s">
-        <v>73</v>
-      </c>
-      <c r="B90" s="75">
-        <f>B88-B89</f>
-        <v>5.6167808629896676</v>
-      </c>
-      <c r="C90" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="E90" s="37"/>
-    </row>
-    <row r="91" spans="1:5">
-      <c r="A91" s="29" t="s">
-        <v>93</v>
-      </c>
-      <c r="B91" s="76">
-        <f>B90/B88</f>
-        <v>0.84886910709202956</v>
-      </c>
-      <c r="C91" s="41"/>
-    </row>
-    <row r="92" spans="1:5">
-      <c r="A92" s="70"/>
-      <c r="B92" s="71"/>
-      <c r="C92" s="48"/>
-    </row>
-    <row r="93" spans="1:5">
-      <c r="A93" s="66"/>
-      <c r="B93" s="55"/>
-      <c r="C93" s="29"/>
-    </row>
-    <row r="94" spans="1:5">
-      <c r="A94" s="66"/>
-      <c r="B94" s="55"/>
-      <c r="C94" s="29"/>
-    </row>
-    <row r="95" spans="1:5">
-      <c r="A95" s="72" t="s">
-        <v>97</v>
-      </c>
-      <c r="B95" s="58"/>
-      <c r="C95" s="40"/>
-    </row>
-    <row r="96" spans="1:5">
-      <c r="A96" s="73" t="s">
-        <v>75</v>
-      </c>
-      <c r="B96" s="55"/>
-      <c r="C96" s="41"/>
-    </row>
-    <row r="97" spans="1:9">
-      <c r="A97" s="73" t="s">
-        <v>76</v>
-      </c>
-      <c r="B97" s="55"/>
-      <c r="C97" s="41"/>
+      <c r="B97" s="54"/>
+      <c r="C97" s="40"/>
     </row>
     <row r="98" spans="1:9">
-      <c r="A98" s="54"/>
-      <c r="B98" s="55"/>
-      <c r="C98" s="41"/>
+      <c r="A98" s="53"/>
+      <c r="B98" s="54"/>
+      <c r="C98" s="40"/>
     </row>
     <row r="99" spans="1:9">
-      <c r="A99" s="56" t="s">
-        <v>46</v>
+      <c r="A99" s="55" t="s">
+        <v>44</v>
       </c>
       <c r="B99" s="12">
         <f>24*365/12</f>
         <v>730</v>
       </c>
-      <c r="C99" s="41" t="s">
+      <c r="C99" s="40" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9">
+      <c r="A100" s="24" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="100" spans="1:9">
-      <c r="A100" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="B100" s="67">
+      <c r="B100" s="66">
         <v>1</v>
       </c>
-      <c r="C100" s="41"/>
+      <c r="C100" s="40"/>
       <c r="E100" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="101" spans="1:9">
-      <c r="A101" s="54" t="s">
-        <v>80</v>
-      </c>
-      <c r="B101" s="59">
+      <c r="A101" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="B101" s="58">
         <f>B99*B100</f>
         <v>730</v>
       </c>
-      <c r="C101" s="41" t="s">
-        <v>45</v>
+      <c r="C101" s="40" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="102" spans="1:9">
-      <c r="A102" s="47"/>
+      <c r="A102" s="46"/>
       <c r="B102" s="6"/>
-      <c r="C102" s="48"/>
+      <c r="C102" s="47"/>
     </row>
     <row r="103" spans="1:9">
-      <c r="A103" s="81"/>
+      <c r="A103" s="80"/>
     </row>
     <row r="105" spans="1:9">
-      <c r="A105" s="24" t="s">
-        <v>82</v>
+      <c r="A105" s="23" t="s">
+        <v>80</v>
       </c>
       <c r="B105" s="4"/>
-      <c r="C105" s="40"/>
+      <c r="C105" s="39"/>
     </row>
     <row r="106" spans="1:9">
-      <c r="A106" s="79" t="s">
-        <v>91</v>
+      <c r="A106" s="78" t="s">
+        <v>89</v>
       </c>
       <c r="B106" s="2"/>
-      <c r="C106" s="41"/>
+      <c r="C106" s="40"/>
       <c r="G106" s="3"/>
       <c r="I106" s="3"/>
     </row>
     <row r="107" spans="1:9">
-      <c r="A107" s="79" t="s">
-        <v>92</v>
+      <c r="A107" s="78" t="s">
+        <v>90</v>
       </c>
       <c r="B107" s="2"/>
-      <c r="C107" s="41"/>
+      <c r="C107" s="40"/>
       <c r="G107" s="3"/>
       <c r="I107" s="3"/>
     </row>
     <row r="108" spans="1:9">
-      <c r="A108" s="61"/>
+      <c r="A108" s="60"/>
       <c r="B108" s="2"/>
-      <c r="C108" s="41"/>
+      <c r="C108" s="40"/>
     </row>
     <row r="109" spans="1:9">
-      <c r="A109" s="49" t="s">
-        <v>83</v>
-      </c>
-      <c r="B109" s="77">
+      <c r="A109" s="48" t="s">
+        <v>81</v>
+      </c>
+      <c r="B109" s="76">
         <f>B101</f>
         <v>730</v>
       </c>
-      <c r="C109" s="41" t="s">
-        <v>45</v>
+      <c r="C109" s="40" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="110" spans="1:9">
-      <c r="A110" s="61"/>
+      <c r="A110" s="60"/>
       <c r="B110" s="2"/>
-      <c r="C110" s="41"/>
+      <c r="C110" s="40"/>
     </row>
     <row r="111" spans="1:9">
-      <c r="A111" s="82" t="s">
-        <v>66</v>
+      <c r="A111" s="81" t="s">
+        <v>64</v>
       </c>
       <c r="B111" s="2">
         <f>B109*B48</f>
-        <v>4830.2500299824569</v>
-      </c>
-      <c r="C111" s="41" t="s">
+        <v>1210.8655746923037</v>
+      </c>
+      <c r="C111" s="40" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="112" spans="1:9">
-      <c r="A112" s="57" t="s">
-        <v>98</v>
+      <c r="A112" s="56" t="s">
+        <v>96</v>
       </c>
       <c r="B112" s="2">
         <f>B109*B58</f>
-        <v>730</v>
-      </c>
-      <c r="C112" s="41" t="s">
+        <v>1886.3200000000002</v>
+      </c>
+      <c r="C112" s="40" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="113" spans="1:3">
-      <c r="A113" s="57" t="s">
-        <v>67</v>
+      <c r="A113" s="56" t="s">
+        <v>65</v>
       </c>
       <c r="B113" s="2">
         <f>B109*B78</f>
         <v>0</v>
       </c>
-      <c r="C113" s="41" t="s">
+      <c r="C113" s="40" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="114" spans="1:3">
-      <c r="A114" s="56" t="s">
-        <v>73</v>
+      <c r="A114" s="55" t="s">
+        <v>71</v>
       </c>
       <c r="B114" s="4">
         <f>B111-B112-B113</f>
-        <v>4100.2500299824569</v>
-      </c>
-      <c r="C114" s="41" t="s">
+        <v>-675.45442530769651</v>
+      </c>
+      <c r="C114" s="40" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="115" spans="1:3">
-      <c r="A115" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="B115" s="77">
+      <c r="A115" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B115" s="76">
         <f>B68</f>
         <v>0</v>
       </c>
-      <c r="C115" s="41" t="s">
+      <c r="C115" s="40" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="116" spans="1:3">
-      <c r="A116" s="80" t="s">
-        <v>90</v>
-      </c>
-      <c r="B116" s="78">
+      <c r="A116" s="79" t="s">
+        <v>88</v>
+      </c>
+      <c r="B116" s="77">
         <f>B114-B115</f>
-        <v>4100.2500299824569</v>
-      </c>
-      <c r="C116" s="41" t="s">
+        <v>-675.45442530769651</v>
+      </c>
+      <c r="C116" s="40" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="117" spans="1:3">
-      <c r="A117" s="47"/>
+      <c r="A117" s="46"/>
       <c r="B117" s="6"/>
-      <c r="C117" s="48"/>
+      <c r="C117" s="47"/>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" s="3"/>
-      <c r="C119" s="30"/>
+      <c r="C119" s="29"/>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" s="3"/>
       <c r="B120" s="2"/>
-      <c r="C120" s="29"/>
+      <c r="C120" s="28"/>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" s="1"/>

</xml_diff>